<commit_message>
BOM completed. Ordering PCB and parts
</commit_message>
<xml_diff>
--- a/assembly/nix-pill-v1.xlsx
+++ b/assembly/nix-pill-v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zuchlewskin\kicad\nix-pill-v1\assembly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B28032-89AB-48AD-B9CC-D2146D0280DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3393A1-47C0-486B-A233-6588E278AE81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="106">
   <si>
     <t>Designator</t>
   </si>
@@ -65,9 +65,6 @@
     <t>100n</t>
   </si>
   <si>
-    <t>20pF</t>
-  </si>
-  <si>
     <t>C7</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
     <t>R9</t>
   </si>
   <si>
-    <t>10M</t>
-  </si>
-  <si>
     <t>SW1</t>
   </si>
   <si>
@@ -333,6 +327,27 @@
   </si>
   <si>
     <t>CC5V-T1A-32.768KHZ-9PF-20PPM-TA-QC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/micro-crystal-ag/CC5V-T1A-32-768KHZ-9PF-20PPM-TA-QC/10499123?s=N4IgTCBcDaIMJwKwDUC0AVAjAQVQZjADoB2ANgA4BpACQC1UBOABQDFUwAGJpgWQ1wCKcEAF0AvkA</t>
+  </si>
+  <si>
+    <t>8pF</t>
+  </si>
+  <si>
+    <t>C1608CH2A080D080AA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/tdk-corporation/C1608CH2A080D080AA/3948350</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/te-connectivity-passive-product/CPF0603B1M0E1/2389636</t>
+  </si>
+  <si>
+    <t>CPF0603B1M0E1</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -1221,7 +1236,7 @@
     <col min="5" max="5" width="34.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="124.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="186.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1264,7 +1279,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F2" s="2">
         <v>0.1</v>
@@ -1274,12 +1289,12 @@
         <v>0.70000000000000007</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>9</v>
@@ -1288,17 +1303,25 @@
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="4"/>
+        <v>100</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.17</v>
+      </c>
       <c r="G3" s="2">
         <f t="shared" ref="G3:G25" si="0">(F3*C3)</f>
-        <v>0</v>
+        <v>0.34</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>9</v>
@@ -1307,10 +1330,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="F4" s="2">
         <v>0.17</v>
@@ -1320,15 +1343,15 @@
         <v>0.34</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -1347,24 +1370,24 @@
         <v>0.17</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F6" s="2">
         <v>0.25</v>
@@ -1374,24 +1397,24 @@
         <v>0.25</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="F7" s="2">
         <v>0.24</v>
@@ -1401,24 +1424,24 @@
         <v>0.24</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" s="2">
         <v>0.24</v>
@@ -1428,24 +1451,24 @@
         <v>0.24</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="F9" s="2">
         <v>0.14000000000000001</v>
@@ -1455,21 +1478,21 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="4">
         <v>22284205</v>
@@ -1482,21 +1505,21 @@
         <v>1.17</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="4">
         <v>877580650</v>
@@ -1509,21 +1532,21 @@
         <v>0.44</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="4">
         <v>1</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="4">
         <v>22284205</v>
@@ -1536,24 +1559,24 @@
         <v>1.17</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="C13" s="4">
         <v>1</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F13" s="2">
         <v>0.45</v>
@@ -1563,24 +1586,24 @@
         <v>0.45</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="C14" s="4">
         <v>1</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="F14" s="2">
         <v>0.75</v>
@@ -1590,15 +1613,15 @@
         <v>0.75</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="C15" s="4">
         <v>2</v>
@@ -1607,7 +1630,7 @@
         <v>100</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F15" s="2">
         <v>0.17</v>
@@ -1617,24 +1640,24 @@
         <v>0.34</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="4">
         <v>3</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F16" s="2">
         <v>0.17</v>
@@ -1644,24 +1667,24 @@
         <v>0.51</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" s="4">
         <v>1</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F17" s="2">
         <v>0.17</v>
@@ -1671,15 +1694,15 @@
         <v>0.17</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="4">
         <v>2</v>
@@ -1688,7 +1711,7 @@
         <v>22</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F18" s="2">
         <v>0.1</v>
@@ -1698,43 +1721,51 @@
         <v>0.2</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="4">
         <v>1</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="4"/>
+        <v>103</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.59</v>
+      </c>
       <c r="G19" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.59</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C20" s="4">
         <v>1</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F20" s="2">
         <v>0.18</v>
@@ -1744,24 +1775,24 @@
         <v>0.18</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C21" s="4">
         <v>1</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F21" s="2">
         <v>0.18</v>
@@ -1771,24 +1802,24 @@
         <v>0.18</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C22" s="4">
         <v>1</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F22" s="2">
         <v>0.41</v>
@@ -1798,24 +1829,24 @@
         <v>0.41</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C23" s="4">
         <v>1</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F23" s="2">
         <v>5.77</v>
@@ -1825,42 +1856,51 @@
         <v>5.77</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C24" s="4">
         <v>1</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="H24" s="1"/>
+        <v>98</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1.18</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>1.18</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C25" s="4">
         <v>1</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F25" s="2">
         <v>0.82</v>
@@ -1870,7 +1910,7 @@
         <v>0.82</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -1884,7 +1924,7 @@
       </c>
       <c r="G26" s="2">
         <f>SUM(G2:G25)</f>
-        <v>14.639999999999999</v>
+        <v>16.75</v>
       </c>
     </row>
   </sheetData>
@@ -1911,8 +1951,10 @@
     <hyperlink ref="H5" r:id="rId19" xr:uid="{7FC0C382-EF09-4636-B74D-49ABBCF89956}"/>
     <hyperlink ref="H25" r:id="rId20" xr:uid="{CE4A456D-1481-41FA-9FAE-3BC7B79A5932}"/>
     <hyperlink ref="H4" r:id="rId21" xr:uid="{642461F8-9E03-40EE-943C-B66BB0EAA464}"/>
+    <hyperlink ref="H3" r:id="rId22" xr:uid="{55CB53C0-0FB2-497D-BF95-77A131696B1E}"/>
+    <hyperlink ref="H19" r:id="rId23" xr:uid="{4B5E1A64-E97C-484C-B51E-E876EBE0339A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>